<commit_message>
Atualizei novamente a planilia de preço (BOM)
Só editei na questão visual
</commit_message>
<xml_diff>
--- a/Excel - Planilia preço.xlsx
+++ b/Excel - Planilia preço.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yure1\OneDrive\Área de Trabalho\UFERSA\Circuito Eletronico 2\Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C486B159-BB48-47EE-8A0B-1CB1750CAB10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACD2925-E6F0-4AD2-9DF2-C695EDA09D3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{59C13A1A-EC07-4893-A243-E3403310A188}"/>
   </bookViews>
@@ -39,15 +39,9 @@
     <t>Dispositivo</t>
   </si>
   <si>
-    <t>Preço</t>
-  </si>
-  <si>
     <t>Quantidade</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Resistor 3.6K</t>
   </si>
   <si>
@@ -109,16 +103,23 @@
   </si>
   <si>
     <t>Potenciomêtro 30K</t>
+  </si>
+  <si>
+    <t>Preço (R$)</t>
+  </si>
+  <si>
+    <t>Total (R$)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +129,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -157,13 +165,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -172,12 +180,6 @@
     <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="6">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -189,22 +191,88 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <numFmt numFmtId="166" formatCode="&quot;R$&quot;\ #,##0.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -221,15 +289,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A69E119-38B6-4DBC-AD71-E2A1547A4F7F}" name="Tabela1" displayName="Tabela1" ref="A1:D23" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A69E119-38B6-4DBC-AD71-E2A1547A4F7F}" name="Tabela1" displayName="Tabela1" ref="A1:D23" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="A1:D23" xr:uid="{4E651197-6098-4168-9F74-62A834BC46A9}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{3945D59D-863C-48F7-9BE1-2B450EF1D2F9}" name="Dispositivo" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{8003C392-6828-41B0-BA80-904BA6C2AB43}" name="Preço" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{C4D4D2DA-8785-43EB-94E8-4AC52E907973}" name="Quantidade" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{D204FCE3-225B-4337-81D6-D2F49D20083F}" name="Total" dataDxfId="2" dataCellStyle="Vírgula"/>
+    <tableColumn id="2" xr3:uid="{8003C392-6828-41B0-BA80-904BA6C2AB43}" name="Preço (R$)" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{C4D4D2DA-8785-43EB-94E8-4AC52E907973}" name="Quantidade" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{D204FCE3-225B-4337-81D6-D2F49D20083F}" name="Total (R$)" dataDxfId="0" dataCellStyle="Vírgula"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -532,36 +600,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFC82452-2709-48FB-A844-2FEA4C7AB7E4}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
     <col min="4" max="4" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3">
         <v>1.9</v>
       </c>
       <c r="C2" s="1">
@@ -572,41 +641,41 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3">
         <v>0.04</v>
       </c>
       <c r="C3" s="1">
         <v>6</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D22" si="0">B3*C3</f>
+        <f>B3*C3</f>
         <v>0.24</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3">
         <v>0.04</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
       </c>
       <c r="D4" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D3:D22" si="0">B4*C4</f>
         <v>0.08</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3">
         <v>0.04</v>
       </c>
       <c r="C5" s="1">
@@ -617,131 +686,131 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.64</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B11" s="3">
         <v>0.04</v>
       </c>
-      <c r="C6" s="1">
-        <v>2</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2">
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1">
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3">
         <v>0.04</v>
       </c>
-      <c r="C7" s="1">
-        <v>2</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2">
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="C8" s="1">
-        <v>2</v>
-      </c>
-      <c r="D8" s="2">
-        <f t="shared" si="0"/>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2</v>
-      </c>
-      <c r="D9" s="2">
-        <f t="shared" si="0"/>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0.64</v>
-      </c>
-      <c r="C10" s="1">
-        <v>2</v>
-      </c>
-      <c r="D10" s="2">
-        <f t="shared" si="0"/>
-        <v>1.28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="B13" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="C11" s="1">
-        <v>2</v>
-      </c>
-      <c r="D11" s="2">
-        <f t="shared" si="0"/>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="C12" s="1">
-        <v>2</v>
-      </c>
-      <c r="D12" s="2">
-        <f t="shared" si="0"/>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="C13" s="1">
-        <v>2</v>
-      </c>
-      <c r="D13" s="2">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="1">
+      <c r="B14" s="3">
         <v>0.28999999999999998</v>
       </c>
       <c r="C14" s="1">
@@ -752,11 +821,11 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="1">
+        <v>16</v>
+      </c>
+      <c r="B15" s="3">
         <v>0.05</v>
       </c>
       <c r="C15" s="1">
@@ -767,11 +836,11 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="1">
+        <v>17</v>
+      </c>
+      <c r="B16" s="3">
         <v>0.05</v>
       </c>
       <c r="C16" s="1">
@@ -782,11 +851,11 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="1">
+        <v>10</v>
+      </c>
+      <c r="B17" s="3">
         <v>0.06</v>
       </c>
       <c r="C17" s="1">
@@ -797,41 +866,41 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="1">
-        <v>0.09</v>
-      </c>
-      <c r="C18" s="1">
-        <v>2</v>
-      </c>
-      <c r="D18" s="2">
-        <f t="shared" si="0"/>
-        <v>0.18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="C19" s="1">
-        <v>2</v>
-      </c>
-      <c r="D19" s="2">
-        <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="1">
+      <c r="B20" s="3">
         <v>1.41</v>
       </c>
       <c r="C20" s="1">
@@ -842,11 +911,11 @@
         <v>9.8699999999999992</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="1">
+        <v>22</v>
+      </c>
+      <c r="B21" s="3">
         <v>25.34</v>
       </c>
       <c r="C21" s="1">
@@ -857,11 +926,11 @@
         <v>76.02</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3">
         <v>1.0900000000000001</v>
       </c>
       <c r="C22" s="1">
@@ -872,11 +941,11 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D23" s="3">
         <f>SUM(D2:D22)</f>

</xml_diff>